<commit_message>
The Cbox is pretty much done.
</commit_message>
<xml_diff>
--- a/doc/CommandsToSysDc Mapping.xlsx
+++ b/doc/CommandsToSysDc Mapping.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="55">
   <si>
     <t>LDx</t>
   </si>
@@ -166,6 +166,21 @@
   </si>
   <si>
     <t>Command</t>
+  </si>
+  <si>
+    <t>Cammand Category</t>
+  </si>
+  <si>
+    <t>Rdx</t>
+  </si>
+  <si>
+    <t>Rdiox</t>
+  </si>
+  <si>
+    <t>RdBlkModx</t>
+  </si>
+  <si>
+    <t>ChxToDirty</t>
   </si>
 </sst>
 </file>
@@ -517,70 +532,76 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:N21"/>
+  <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="18.42578125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="17.42578125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.7109375" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="9.42578125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="13.85546875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.7109375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="10" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="17.42578125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="9.42578125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.140625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14">
+    <row r="1" spans="1:15">
       <c r="B1" s="2" t="s">
         <v>49</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>48</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="L1" s="2" t="s">
+      <c r="M1" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="M1" s="2" t="s">
+      <c r="N1" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="N1" s="2" t="s">
+      <c r="O1" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:14">
+    <row r="2" spans="1:15">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -588,23 +609,23 @@
         <v>1</v>
       </c>
       <c r="C2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2" s="1"/>
       <c r="F2" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H2" s="1"/>
+      <c r="H2" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="I2" s="1"/>
-      <c r="J2" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
         <v>34</v>
       </c>
@@ -614,9 +635,12 @@
       <c r="M2" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14">
+      <c r="N2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="2" t="s">
         <v>40</v>
       </c>
@@ -624,18 +648,18 @@
         <v>44</v>
       </c>
       <c r="C3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F3" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="D3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="G3" s="4"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4"/>
-      <c r="J3" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="J3" s="4"/>
       <c r="K3" s="4" t="s">
         <v>34</v>
       </c>
@@ -645,8 +669,11 @@
       <c r="M3" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:14">
+      <c r="N3" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="2" t="s">
         <v>41</v>
       </c>
@@ -654,18 +681,18 @@
         <v>44</v>
       </c>
       <c r="C4" t="s">
-        <v>2</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F4" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="D4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="G4" s="4"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4"/>
-      <c r="J4" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="J4" s="4"/>
       <c r="K4" s="4" t="s">
         <v>34</v>
       </c>
@@ -675,8 +702,11 @@
       <c r="M4" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="5" spans="1:14">
+      <c r="N4" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="2" t="s">
         <v>42</v>
       </c>
@@ -684,18 +714,18 @@
         <v>45</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="D5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="G5" s="4"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4"/>
-      <c r="J5" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="J5" s="4"/>
       <c r="K5" s="4" t="s">
         <v>34</v>
       </c>
@@ -705,8 +735,11 @@
       <c r="M5" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="6" spans="1:14">
+      <c r="N5" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="2" t="s">
         <v>43</v>
       </c>
@@ -714,18 +747,18 @@
         <v>46</v>
       </c>
       <c r="C6" t="s">
-        <v>2</v>
-      </c>
-      <c r="E6" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="F6" s="4"/>
+        <v>52</v>
+      </c>
+      <c r="D6" t="s">
+        <v>2</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="G6" s="4"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4"/>
-      <c r="J6" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="J6" s="4"/>
       <c r="K6" s="4" t="s">
         <v>34</v>
       </c>
@@ -735,8 +768,11 @@
       <c r="M6" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="7" spans="1:14">
+      <c r="N6" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
@@ -744,23 +780,23 @@
         <v>4</v>
       </c>
       <c r="C7" t="s">
-        <v>2</v>
-      </c>
-      <c r="D7" s="1"/>
-      <c r="E7" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E7" s="1"/>
       <c r="F7" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H7" s="1"/>
+      <c r="H7" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="I7" s="1"/>
-      <c r="J7" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
         <v>34</v>
       </c>
@@ -770,9 +806,12 @@
       <c r="M7" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14">
+      <c r="N7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -780,23 +819,23 @@
         <v>4</v>
       </c>
       <c r="C8" t="s">
-        <v>2</v>
-      </c>
-      <c r="D8" s="1"/>
-      <c r="E8" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>53</v>
+      </c>
+      <c r="D8" t="s">
+        <v>2</v>
+      </c>
+      <c r="E8" s="1"/>
       <c r="F8" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H8" s="1"/>
+      <c r="H8" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="I8" s="1"/>
-      <c r="J8" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="J8" s="1"/>
       <c r="K8" s="1" t="s">
         <v>34</v>
       </c>
@@ -806,9 +845,12 @@
       <c r="M8" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14">
+      <c r="N8" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="2" t="s">
         <v>15</v>
       </c>
@@ -816,23 +858,23 @@
         <v>16</v>
       </c>
       <c r="C9" t="s">
-        <v>2</v>
-      </c>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>51</v>
+      </c>
+      <c r="D9" t="s">
+        <v>2</v>
+      </c>
+      <c r="E9" s="1"/>
       <c r="F9" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H9" s="1"/>
+      <c r="H9" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="I9" s="1"/>
-      <c r="J9" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
         <v>34</v>
       </c>
@@ -842,9 +884,12 @@
       <c r="M9" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14">
+      <c r="N9" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="2" t="s">
         <v>6</v>
       </c>
@@ -852,23 +897,23 @@
         <v>7</v>
       </c>
       <c r="C10" t="s">
-        <v>2</v>
-      </c>
-      <c r="D10" s="1"/>
-      <c r="E10" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D10" t="s">
+        <v>2</v>
+      </c>
+      <c r="E10" s="1"/>
       <c r="F10" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H10" s="1"/>
+      <c r="H10" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="I10" s="1"/>
-      <c r="J10" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="J10" s="1"/>
       <c r="K10" s="1" t="s">
         <v>34</v>
       </c>
@@ -878,9 +923,12 @@
       <c r="M10" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14">
+      <c r="N10" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
@@ -888,23 +936,23 @@
         <v>8</v>
       </c>
       <c r="C11" t="s">
-        <v>2</v>
-      </c>
-      <c r="D11" s="1"/>
-      <c r="E11" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>54</v>
+      </c>
+      <c r="D11" t="s">
+        <v>2</v>
+      </c>
+      <c r="E11" s="1"/>
       <c r="F11" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H11" s="1"/>
+      <c r="H11" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="I11" s="1"/>
-      <c r="J11" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
         <v>34</v>
       </c>
@@ -914,9 +962,12 @@
       <c r="M11" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N11" s="1"/>
-    </row>
-    <row r="12" spans="1:14">
+      <c r="N11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O11" s="1"/>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="2" t="s">
         <v>9</v>
       </c>
@@ -924,23 +975,23 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>2</v>
-      </c>
-      <c r="D12" s="1"/>
-      <c r="E12" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>10</v>
+      </c>
+      <c r="D12" t="s">
+        <v>2</v>
+      </c>
+      <c r="E12" s="1"/>
       <c r="F12" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H12" s="1"/>
+      <c r="H12" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="I12" s="1"/>
-      <c r="J12" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
         <v>34</v>
       </c>
@@ -950,9 +1001,12 @@
       <c r="M12" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N12" s="1"/>
-    </row>
-    <row r="13" spans="1:14">
+      <c r="N12" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12" s="1"/>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -960,23 +1014,23 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
-        <v>2</v>
-      </c>
-      <c r="D13" s="1"/>
-      <c r="E13" s="1" t="s">
-        <v>34</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="D13" t="s">
+        <v>2</v>
+      </c>
+      <c r="E13" s="1"/>
       <c r="F13" s="1" t="s">
         <v>34</v>
       </c>
       <c r="G13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="H13" s="1"/>
+      <c r="H13" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="I13" s="1"/>
-      <c r="J13" s="1" t="s">
-        <v>34</v>
-      </c>
+      <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
         <v>34</v>
       </c>
@@ -986,9 +1040,12 @@
       <c r="M13" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="N13" s="1"/>
-    </row>
-    <row r="14" spans="1:14">
+      <c r="N13" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="O13" s="1"/>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="2" t="s">
         <v>13</v>
       </c>
@@ -996,81 +1053,92 @@
         <v>14</v>
       </c>
       <c r="C14" t="s">
-        <v>2</v>
-      </c>
-      <c r="D14" s="1"/>
+        <v>14</v>
+      </c>
+      <c r="D14" t="s">
+        <v>2</v>
+      </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
-      <c r="G14" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="H14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1" t="s">
+        <v>34</v>
+      </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1"/>
       <c r="L14" s="1"/>
       <c r="M14" s="1"/>
       <c r="N14" s="1"/>
-    </row>
-    <row r="15" spans="1:14">
-      <c r="A15" s="6" t="s">
+      <c r="O14" s="1"/>
+    </row>
+    <row r="15" spans="1:15">
+      <c r="A15" s="2"/>
+      <c r="B15" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" t="s">
+        <v>28</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="E15" s="4"/>
+      <c r="F15" s="4"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J15" s="4"/>
+      <c r="K15" s="4"/>
+      <c r="L15" s="4"/>
+      <c r="M15" s="4"/>
+      <c r="N15" s="4"/>
+      <c r="O15" s="4"/>
+    </row>
+    <row r="16" spans="1:15">
+      <c r="A16" s="2"/>
+      <c r="B16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="3"/>
+      <c r="H16" s="3"/>
+      <c r="I16" s="3"/>
+      <c r="J16" s="3"/>
+      <c r="K16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="M16" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="N16" s="3" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
+      <c r="A17" s="6" t="s">
         <v>47</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B17" t="s">
         <v>17</v>
       </c>
-      <c r="C15" t="s">
+      <c r="D17" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="1"/>
-      <c r="E15" s="1"/>
-      <c r="F15" s="1"/>
-      <c r="G15" s="1"/>
-      <c r="H15" s="1"/>
-      <c r="I15" s="1"/>
-      <c r="J15" s="1"/>
-      <c r="K15" s="1"/>
-      <c r="L15" s="1"/>
-      <c r="M15" s="1"/>
-      <c r="N15" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="16" spans="1:14">
-      <c r="A16" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
-      </c>
-      <c r="C16" t="s">
-        <v>20</v>
-      </c>
-      <c r="D16" s="1"/>
-      <c r="E16" s="1"/>
-      <c r="F16" s="1"/>
-      <c r="G16" s="1"/>
-      <c r="H16" s="1"/>
-      <c r="I16" s="1"/>
-      <c r="J16" s="1"/>
-      <c r="K16" s="1"/>
-      <c r="L16" s="1"/>
-      <c r="M16" s="1"/>
-      <c r="N16" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="17" spans="1:14">
-      <c r="A17" s="2" t="s">
-        <v>37</v>
-      </c>
-      <c r="B17" t="s">
-        <v>19</v>
-      </c>
-      <c r="C17" t="s">
-        <v>20</v>
-      </c>
-      <c r="D17" s="1"/>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
       <c r="G17" s="1"/>
@@ -1080,21 +1148,21 @@
       <c r="K17" s="1"/>
       <c r="L17" s="1"/>
       <c r="M17" s="1"/>
-      <c r="N17" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14">
+      <c r="N17" s="1"/>
+      <c r="O17" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="2" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18" t="s">
         <v>20</v>
       </c>
-      <c r="D18" s="1"/>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
       <c r="G18" s="1"/>
@@ -1104,21 +1172,21 @@
       <c r="K18" s="1"/>
       <c r="L18" s="1"/>
       <c r="M18" s="1"/>
-      <c r="N18" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14">
+      <c r="N18" s="1"/>
+      <c r="O18" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="2" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" t="s">
-        <v>22</v>
-      </c>
-      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
         <v>20</v>
       </c>
-      <c r="D19" s="1"/>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
       <c r="G19" s="1"/>
@@ -1128,58 +1196,56 @@
       <c r="K19" s="1"/>
       <c r="L19" s="1"/>
       <c r="M19" s="1"/>
-      <c r="N19" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14">
-      <c r="A20" s="2"/>
-      <c r="B20" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="I20" s="4"/>
-      <c r="J20" s="4"/>
-      <c r="K20" s="4"/>
-      <c r="L20" s="4"/>
-      <c r="M20" s="4"/>
-      <c r="N20" s="4"/>
-    </row>
-    <row r="21" spans="1:14">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2" t="s">
-        <v>35</v>
-      </c>
-      <c r="C21" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="F21" s="3"/>
-      <c r="G21" s="3"/>
-      <c r="H21" s="3"/>
-      <c r="I21" s="3"/>
-      <c r="J21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="K21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="L21" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="M21" s="3" t="s">
+      <c r="N19" s="1"/>
+      <c r="O19" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
+      <c r="A20" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="1"/>
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+      <c r="I20" s="1"/>
+      <c r="J20" s="1"/>
+      <c r="K20" s="1"/>
+      <c r="L20" s="1"/>
+      <c r="M20" s="1"/>
+      <c r="N20" s="1"/>
+      <c r="O20" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
+      <c r="A21" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="1"/>
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+      <c r="I21" s="1"/>
+      <c r="J21" s="1"/>
+      <c r="K21" s="1"/>
+      <c r="L21" s="1"/>
+      <c r="M21" s="1"/>
+      <c r="N21" s="1"/>
+      <c r="O21" s="1" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>